<commit_message>
# add program xxptrp07.p.
</commit_message>
<xml_diff>
--- a/vst/cim.xlsx
+++ b/vst/cim.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="100">
   <si>
     <t>gplbldmt.p</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -246,6 +246,98 @@
   </si>
   <si>
     <t>YIELD_PERCENT</t>
+  </si>
+  <si>
+    <t>t_lddet_loc</t>
+  </si>
+  <si>
+    <t>t_lddet_part</t>
+  </si>
+  <si>
+    <t>pt_desc1</t>
+  </si>
+  <si>
+    <t>pt_draw</t>
+  </si>
+  <si>
+    <t>t_sct_abc</t>
+  </si>
+  <si>
+    <t>t_lddet_qty</t>
+  </si>
+  <si>
+    <t>t_sct_um</t>
+  </si>
+  <si>
+    <t>ext_std</t>
+  </si>
+  <si>
+    <t>t_part_type</t>
+  </si>
+  <si>
+    <t>t_acct</t>
+  </si>
+  <si>
+    <t>t_sub</t>
+  </si>
+  <si>
+    <t>xxptrp07.p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SITE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOCATION</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEM_NUMBER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DRAWING</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>ABC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNITS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QUANTITY_ON_HAND</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACCTS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUB-ACCOUNT</t>
+  </si>
+  <si>
+    <t>GL_COST</t>
+  </si>
+  <si>
+    <t>GL_COST_TOTAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_sct_std_as_of</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>in_site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -601,11 +693,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -851,6 +943,149 @@
       </c>
       <c r="C29" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>